<commit_message>
first commit cover main done 2
</commit_message>
<xml_diff>
--- a/cover_data.xlsx
+++ b/cover_data.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\0_Python\pydocx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{219AC270-DDD1-48F3-AABD-2C7FD103C86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C3B807-401E-4C8D-8E16-9619AD73E718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{CF1D6D8B-DEB8-4CAF-9326-0A70C5378741}"/>
   </bookViews>
   <sheets>
     <sheet name="cover_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>&lt;ANNEX-ID&gt;</t>
   </si>
@@ -56,6 +69,9 @@
   </si>
   <si>
     <t>&lt;ANNEX-SUB-NO&gt;</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -539,8 +555,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -919,13 +936,17 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -985,8 +1006,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>

</xml_diff>